<commit_message>
Uppfærði excelskjalid, saveaði aftur sem stadavika3
</commit_message>
<xml_diff>
--- a/stadavika2.xlsx
+++ b/stadavika2.xlsx
@@ -812,27 +812,27 @@
                   <c:v>3630</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3630</c:v>
+                  <c:v>3130</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3630</c:v>
+                  <c:v>2330</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3630</c:v>
+                  <c:v>1310</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3630</c:v>
+                  <c:v>1310</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="116514176"/>
-        <c:axId val="120525952"/>
+        <c:axId val="132398464"/>
+        <c:axId val="134468736"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="116514176"/>
+        <c:axId val="132398464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -840,14 +840,14 @@
         <c:numFmt formatCode="d/m/yyyy" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="120525952"/>
+        <c:crossAx val="134468736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="120525952"/>
+        <c:axId val="134468736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -861,7 +861,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="116514176"/>
+        <c:crossAx val="132398464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -913,7 +913,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1098,11 +1098,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="78892416"/>
-        <c:axId val="135245184"/>
+        <c:axId val="133703168"/>
+        <c:axId val="133704704"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="78892416"/>
+        <c:axId val="133703168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1110,14 +1110,14 @@
         <c:numFmt formatCode="d/m/yyyy" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="135245184"/>
+        <c:crossAx val="133704704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="135245184"/>
+        <c:axId val="133704704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1131,7 +1131,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="78892416"/>
+        <c:crossAx val="133703168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1183,7 +1183,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1355,18 +1355,18 @@
                   <c:v>1740</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>720</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="50476160"/>
-        <c:axId val="50524544"/>
+        <c:axId val="133721472"/>
+        <c:axId val="133739648"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="50476160"/>
+        <c:axId val="133721472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1374,14 +1374,14 @@
         <c:numFmt formatCode="d/m/yyyy" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50524544"/>
+        <c:crossAx val="133739648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="50524544"/>
+        <c:axId val="133739648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1395,7 +1395,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="50476160"/>
+        <c:crossAx val="133721472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1447,7 +1447,269 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000144" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000144" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="is-IS"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="is-IS"/>
+              <a:t>Ítrun</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="is-IS" baseline="0"/>
+              <a:t> 3</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Tími eftir</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Notendasögur!$J$55:$J$61</c:f>
+              <c:numCache>
+                <c:formatCode>d/m/yyyy</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>41683</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>41684</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41685</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>41686</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>41687</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>41688</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>41689</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Notendasögur!$G$55:$G$61</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>720</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>480</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Rauntími eftir</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Notendasögur!$J$55:$J$61</c:f>
+              <c:numCache>
+                <c:formatCode>d/m/yyyy</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>41683</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>41684</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41685</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>41686</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>41687</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>41688</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>41689</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Notendasögur!$H$56:$H$62</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>720</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>720</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>720</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>720</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>720</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="143396864"/>
+        <c:axId val="143398400"/>
+      </c:lineChart>
+      <c:dateAx>
+        <c:axId val="143396864"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="d/m/yyyy" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="143398400"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="days"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="143398400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="9525">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="143396864"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="span"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:srgbClr val="5E9EFF"/>
+        </a:gs>
+        <a:gs pos="39999">
+          <a:srgbClr val="85C2FF"/>
+        </a:gs>
+        <a:gs pos="70000">
+          <a:srgbClr val="C4D6EB"/>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:srgbClr val="FFEBFA"/>
+        </a:gs>
+      </a:gsLst>
+      <a:lin ang="2700000" scaled="0"/>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln cap="rnd" cmpd="dbl">
+      <a:solidFill>
+        <a:schemeClr val="tx1"/>
+      </a:solidFill>
+    </a:ln>
+    <a:effectLst>
+      <a:innerShdw blurRad="114300">
+        <a:prstClr val="black"/>
+      </a:innerShdw>
+    </a:effectLst>
+    <a:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </a:scene3d>
+    <a:sp3d>
+      <a:bevelT/>
+      <a:bevelB/>
+    </a:sp3d>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000167" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000167" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1540,6 +1802,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>593889</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1847,8 +2139,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C13" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="G48" sqref="G48"/>
+    <sheetView tabSelected="1" topLeftCell="B12" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2238,10 +2530,10 @@
       </c>
       <c r="H14" s="6">
         <f t="shared" si="0"/>
-        <v>3630</v>
+        <v>3130</v>
       </c>
       <c r="I14" s="6">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="J14" s="5">
         <v>41680</v>
@@ -2268,10 +2560,10 @@
       </c>
       <c r="H15" s="6">
         <f t="shared" si="0"/>
-        <v>3630</v>
+        <v>2330</v>
       </c>
       <c r="I15" s="6">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="J15" s="5">
         <v>41681</v>
@@ -2297,10 +2589,10 @@
       </c>
       <c r="H16" s="6">
         <f>H15-I16</f>
-        <v>3630</v>
+        <v>1310</v>
       </c>
       <c r="I16" s="6">
-        <v>0</v>
+        <v>1020</v>
       </c>
       <c r="J16" s="5">
         <v>41682</v>
@@ -2320,7 +2612,7 @@
       <c r="E17" s="10"/>
       <c r="H17" s="6">
         <f>H16-I17</f>
-        <v>3630</v>
+        <v>1310</v>
       </c>
       <c r="J17" s="5"/>
     </row>
@@ -2853,8 +3145,7 @@
         <v>540</v>
       </c>
       <c r="H47" s="6">
-        <f t="shared" si="2"/>
-        <v>720</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:10">
@@ -2872,7 +3163,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:10">
       <c r="A49" s="19">
         <v>30</v>
       </c>
@@ -2883,7 +3174,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:10">
       <c r="A50" s="19">
         <v>31</v>
       </c>
@@ -2894,7 +3185,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:10">
       <c r="A52" s="14"/>
       <c r="B52" s="14" t="s">
         <v>73</v>
@@ -2903,12 +3194,12 @@
         <v>540</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:10">
       <c r="A53" s="14"/>
       <c r="B53" s="14"/>
       <c r="C53" s="14"/>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:10">
       <c r="A55" s="22"/>
       <c r="B55" s="23" t="s">
         <v>7</v>
@@ -2917,8 +3208,20 @@
         <f>C56</f>
         <v>240</v>
       </c>
-    </row>
-    <row r="56" spans="1:3">
+      <c r="G55" s="6">
+        <v>720</v>
+      </c>
+      <c r="H55" s="6">
+        <v>720</v>
+      </c>
+      <c r="I55">
+        <v>0</v>
+      </c>
+      <c r="J55" s="5">
+        <v>41683</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10">
       <c r="A56" s="22">
         <v>21</v>
       </c>
@@ -2928,8 +3231,38 @@
       <c r="C56" s="24">
         <v>240</v>
       </c>
-    </row>
-    <row r="58" spans="1:3">
+      <c r="G56" s="6">
+        <f>G55-G63</f>
+        <v>600</v>
+      </c>
+      <c r="H56" s="6">
+        <f>H55-I55</f>
+        <v>720</v>
+      </c>
+      <c r="I56">
+        <v>0</v>
+      </c>
+      <c r="J56" s="5">
+        <v>41684</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10">
+      <c r="G57" s="6">
+        <f>G56-G63</f>
+        <v>480</v>
+      </c>
+      <c r="H57" s="6">
+        <f>H56-I56</f>
+        <v>720</v>
+      </c>
+      <c r="I57">
+        <v>0</v>
+      </c>
+      <c r="J57" s="5">
+        <v>41685</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10">
       <c r="A58" s="22"/>
       <c r="B58" s="23" t="s">
         <v>3</v>
@@ -2938,8 +3271,22 @@
         <f>SUM(C59,C60)</f>
         <v>360</v>
       </c>
-    </row>
-    <row r="59" spans="1:3">
+      <c r="G58" s="6">
+        <f>G57-G63</f>
+        <v>360</v>
+      </c>
+      <c r="H58" s="6">
+        <f>H57-I57</f>
+        <v>720</v>
+      </c>
+      <c r="I58">
+        <v>0</v>
+      </c>
+      <c r="J58" s="5">
+        <v>41686</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10">
       <c r="A59" s="22">
         <v>23</v>
       </c>
@@ -2949,8 +3296,22 @@
       <c r="C59" s="24">
         <v>180</v>
       </c>
-    </row>
-    <row r="60" spans="1:3">
+      <c r="G59" s="6">
+        <f>G58-G63</f>
+        <v>240</v>
+      </c>
+      <c r="H59" s="6">
+        <f>H58-I58</f>
+        <v>720</v>
+      </c>
+      <c r="I59">
+        <v>0</v>
+      </c>
+      <c r="J59" s="5">
+        <v>41687</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10">
       <c r="A60" s="22">
         <v>25</v>
       </c>
@@ -2960,8 +3321,38 @@
       <c r="C60" s="24">
         <v>180</v>
       </c>
-    </row>
-    <row r="62" spans="1:3">
+      <c r="G60" s="6">
+        <f>G59-G63</f>
+        <v>120</v>
+      </c>
+      <c r="H60" s="6">
+        <f>H59-I59</f>
+        <v>720</v>
+      </c>
+      <c r="I60">
+        <v>720</v>
+      </c>
+      <c r="J60" s="5">
+        <v>41688</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10">
+      <c r="G61" s="6">
+        <f>G60-G63</f>
+        <v>0</v>
+      </c>
+      <c r="H61" s="6">
+        <f>H60-I60</f>
+        <v>0</v>
+      </c>
+      <c r="I61">
+        <v>0</v>
+      </c>
+      <c r="J61" s="5">
+        <v>41689</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10">
       <c r="A62" s="22"/>
       <c r="B62" s="23" t="s">
         <v>72</v>
@@ -2970,8 +3361,12 @@
         <f>C63</f>
         <v>120</v>
       </c>
-    </row>
-    <row r="63" spans="1:3">
+      <c r="H62" s="6">
+        <f>H61-I61</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10">
       <c r="A63" s="22">
         <v>27</v>
       </c>
@@ -2979,6 +3374,10 @@
         <v>67</v>
       </c>
       <c r="C63" s="24">
+        <v>120</v>
+      </c>
+      <c r="G63">
+        <f>G55/6</f>
         <v>120</v>
       </c>
     </row>

</xml_diff>